<commit_message>
Combined Data for Analysis and added numeric values to squad etc for comparision
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Documents\College\FortniteHeatMap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shivanikohli/Desktop/Junior Year/Intro to Data Science/Final project/Fortnite_Heatmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857A406E-F0F9-4BFE-8D2D-97477B6C217B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1ACC57-F8D4-B649-865D-8A5F3BCDDDB1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9636" xr2:uid="{1170DAF0-48DC-4BCD-8C0E-9A90E499DE73}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16240" xr2:uid="{1170DAF0-48DC-4BCD-8C0E-9A90E499DE73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,1802 +510,1802 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E30DA7-F07E-4C05-AD88-335681503F00}">
   <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="D129" sqref="D129"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
       <c r="C3">
         <v>60</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
       <c r="C4">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
       <c r="C5">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" t="s">
+        <v>4</v>
       </c>
       <c r="C6">
         <v>43</v>
       </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" t="s">
+        <v>4</v>
       </c>
       <c r="C7">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
-        <v>1</v>
+      <c r="B8" t="s">
+        <v>4</v>
       </c>
       <c r="C8">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" t="s">
+        <v>4</v>
       </c>
       <c r="C9">
         <v>50</v>
       </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
-        <v>1</v>
+      <c r="B10" t="s">
+        <v>4</v>
       </c>
       <c r="C10">
         <v>47</v>
       </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
-        <v>0</v>
+      <c r="B11" t="s">
+        <v>4</v>
       </c>
       <c r="C11">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B12">
-        <v>0</v>
+      <c r="B12" t="s">
+        <v>4</v>
       </c>
       <c r="C12">
         <v>49</v>
       </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
-        <v>0</v>
+      <c r="B13" t="s">
+        <v>4</v>
       </c>
       <c r="C13">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
-        <v>1</v>
+      <c r="B14" t="s">
+        <v>4</v>
       </c>
       <c r="C14">
         <v>16</v>
       </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>2</v>
+      <c r="B15" t="s">
+        <v>4</v>
       </c>
       <c r="C15">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="B17" t="s">
+        <v>4</v>
       </c>
       <c r="C17">
         <v>25</v>
       </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18">
-        <v>0</v>
+      <c r="B18" t="s">
+        <v>18</v>
       </c>
       <c r="C18">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
-        <v>1</v>
+      <c r="B19" t="s">
+        <v>18</v>
       </c>
       <c r="C19">
         <v>21</v>
       </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="B20" t="s">
+        <v>18</v>
       </c>
       <c r="C20">
         <v>28</v>
       </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
-      <c r="B21">
-        <v>2</v>
+      <c r="B21" t="s">
+        <v>18</v>
       </c>
       <c r="C21">
         <v>13</v>
       </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>0</v>
+      <c r="B22" t="s">
+        <v>20</v>
       </c>
       <c r="C22">
         <v>6</v>
       </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23">
-        <v>1</v>
+      <c r="B23" t="s">
+        <v>18</v>
       </c>
       <c r="C23">
         <v>26</v>
       </c>
-      <c r="D23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B24">
-        <v>1</v>
+      <c r="B24" t="s">
+        <v>6</v>
       </c>
       <c r="C24">
         <v>37</v>
       </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
-      <c r="B25">
-        <v>0</v>
+      <c r="B25" t="s">
+        <v>18</v>
       </c>
       <c r="C25">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
-      <c r="B26">
-        <v>1</v>
+      <c r="B26" t="s">
+        <v>18</v>
       </c>
       <c r="C26">
         <v>13</v>
       </c>
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>21</v>
       </c>
-      <c r="B27">
-        <v>1</v>
+      <c r="B27" t="s">
+        <v>18</v>
       </c>
       <c r="C27">
         <v>25</v>
       </c>
-      <c r="D27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B28">
-        <v>0</v>
+      <c r="B28" t="s">
+        <v>18</v>
       </c>
       <c r="C28">
         <v>22</v>
       </c>
-      <c r="D28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B29">
-        <v>0</v>
+      <c r="B29" t="s">
+        <v>18</v>
       </c>
       <c r="C29">
         <v>22</v>
       </c>
-      <c r="D29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30">
-        <v>3</v>
+      <c r="B30" t="s">
+        <v>18</v>
       </c>
       <c r="C30">
         <v>18</v>
       </c>
-      <c r="D30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
-      <c r="B31">
-        <v>0</v>
+      <c r="B31" t="s">
+        <v>6</v>
       </c>
       <c r="C31">
         <v>15</v>
       </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>7</v>
       </c>
-      <c r="B32">
-        <v>0</v>
+      <c r="B32" t="s">
+        <v>6</v>
       </c>
       <c r="C32">
         <v>27</v>
       </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>24</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
         <v>3</v>
       </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>7</v>
       </c>
-      <c r="B34">
-        <v>0</v>
+      <c r="B34" t="s">
+        <v>4</v>
       </c>
       <c r="C34">
         <v>35</v>
       </c>
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="s">
         <v>4</v>
       </c>
       <c r="C35">
         <v>20</v>
       </c>
-      <c r="D35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>25</v>
       </c>
-      <c r="B36">
-        <v>0</v>
+      <c r="B36" t="s">
+        <v>4</v>
       </c>
       <c r="C36">
         <v>50</v>
       </c>
-      <c r="D36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
-      <c r="B37">
-        <v>0</v>
+      <c r="B37" t="s">
+        <v>4</v>
       </c>
       <c r="C37">
         <v>48</v>
       </c>
-      <c r="D37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>26</v>
       </c>
-      <c r="B38">
-        <v>2</v>
+      <c r="B38" t="s">
+        <v>4</v>
       </c>
       <c r="C38">
         <v>9</v>
       </c>
-      <c r="D38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>
-      <c r="B39">
-        <v>0</v>
+      <c r="B39" t="s">
+        <v>4</v>
       </c>
       <c r="C39">
         <v>34</v>
       </c>
-      <c r="D39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>13</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
         <v>11</v>
       </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>23</v>
       </c>
-      <c r="B41">
-        <v>1</v>
+      <c r="B41" t="s">
+        <v>4</v>
       </c>
       <c r="C41">
         <v>34</v>
       </c>
-      <c r="D41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>19</v>
       </c>
-      <c r="B42">
-        <v>1</v>
+      <c r="B42" t="s">
+        <v>4</v>
       </c>
       <c r="C42">
         <v>8</v>
       </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>27</v>
       </c>
-      <c r="B43">
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
         <v>5</v>
       </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>13</v>
       </c>
-      <c r="B44">
+      <c r="B44" t="s">
         <v>4</v>
       </c>
       <c r="C44">
         <v>30</v>
       </c>
-      <c r="D44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>28</v>
       </c>
-      <c r="B45">
+      <c r="B45" t="s">
         <v>6</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="D45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
-      <c r="B46">
-        <v>0</v>
+      <c r="B46" t="s">
+        <v>4</v>
       </c>
       <c r="C46">
         <v>37</v>
       </c>
-      <c r="D46" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>21</v>
       </c>
-      <c r="B47">
-        <v>0</v>
+      <c r="B47" t="s">
+        <v>4</v>
       </c>
       <c r="C47">
         <v>16</v>
       </c>
-      <c r="D47" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>12</v>
       </c>
-      <c r="B48">
-        <v>2</v>
+      <c r="B48" t="s">
+        <v>4</v>
       </c>
       <c r="C48">
         <v>25</v>
       </c>
-      <c r="D48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>29</v>
       </c>
-      <c r="B49">
-        <v>2</v>
+      <c r="B49" t="s">
+        <v>4</v>
       </c>
       <c r="C49">
         <v>18</v>
       </c>
-      <c r="D49" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>30</v>
       </c>
-      <c r="B50">
-        <v>2</v>
+      <c r="B50" t="s">
+        <v>6</v>
       </c>
       <c r="C50">
         <v>62</v>
       </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>30</v>
       </c>
-      <c r="B51">
-        <v>1</v>
+      <c r="B51" t="s">
+        <v>6</v>
       </c>
       <c r="C51">
         <v>75</v>
       </c>
-      <c r="D51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>14</v>
       </c>
-      <c r="B52">
-        <v>0</v>
+      <c r="B52" t="s">
+        <v>6</v>
       </c>
       <c r="C52">
         <v>24</v>
       </c>
-      <c r="D52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>23</v>
       </c>
-      <c r="B53">
-        <v>0</v>
+      <c r="B53" t="s">
+        <v>6</v>
       </c>
       <c r="C53">
         <v>91</v>
       </c>
-      <c r="D53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>31</v>
       </c>
-      <c r="B54">
-        <v>0</v>
+      <c r="B54" t="s">
+        <v>6</v>
       </c>
       <c r="C54">
         <v>78</v>
       </c>
-      <c r="D54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>24</v>
       </c>
-      <c r="B55">
-        <v>1</v>
+      <c r="B55" t="s">
+        <v>6</v>
       </c>
       <c r="C55">
         <v>30</v>
       </c>
-      <c r="D55" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>25</v>
       </c>
-      <c r="B56">
-        <v>1</v>
+      <c r="B56" t="s">
+        <v>6</v>
       </c>
       <c r="C56">
         <v>12</v>
       </c>
-      <c r="D56" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>32</v>
       </c>
-      <c r="B57">
-        <v>1</v>
+      <c r="B57" t="s">
+        <v>6</v>
       </c>
       <c r="C57">
         <v>4</v>
       </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>7</v>
       </c>
-      <c r="B58">
-        <v>0</v>
+      <c r="B58" t="s">
+        <v>6</v>
       </c>
       <c r="C58">
         <v>67</v>
       </c>
-      <c r="D58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>9</v>
       </c>
-      <c r="B59">
-        <v>0</v>
+      <c r="B59" t="s">
+        <v>6</v>
       </c>
       <c r="C59">
         <v>48</v>
       </c>
-      <c r="D59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>13</v>
       </c>
-      <c r="B60">
-        <v>1</v>
+      <c r="B60" t="s">
+        <v>6</v>
       </c>
       <c r="C60">
         <v>6</v>
       </c>
-      <c r="D60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>9</v>
       </c>
-      <c r="B61">
-        <v>2</v>
+      <c r="B61" t="s">
+        <v>6</v>
       </c>
       <c r="C61">
         <v>24</v>
       </c>
-      <c r="D61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>33</v>
       </c>
-      <c r="B62">
-        <v>0</v>
+      <c r="B62" t="s">
+        <v>4</v>
       </c>
       <c r="C62">
         <v>14</v>
       </c>
-      <c r="D62" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>34</v>
       </c>
-      <c r="B63">
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
         <v>10</v>
       </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>14</v>
       </c>
-      <c r="B64">
-        <v>1</v>
+      <c r="B64" t="s">
+        <v>4</v>
       </c>
       <c r="C64">
         <v>38</v>
       </c>
-      <c r="D64" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>35</v>
       </c>
-      <c r="B65">
-        <v>0</v>
+      <c r="B65" t="s">
+        <v>4</v>
       </c>
       <c r="C65">
         <v>44</v>
       </c>
-      <c r="D65" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>8</v>
       </c>
-      <c r="B66">
-        <v>2</v>
+      <c r="B66" t="s">
+        <v>4</v>
       </c>
       <c r="C66">
         <v>27</v>
       </c>
-      <c r="D66" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>35</v>
       </c>
-      <c r="B67">
-        <v>1</v>
+      <c r="B67" t="s">
+        <v>4</v>
       </c>
       <c r="C67">
         <v>22</v>
       </c>
-      <c r="D67" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>15</v>
       </c>
-      <c r="B68">
-        <v>0</v>
+      <c r="B68" t="s">
+        <v>4</v>
       </c>
       <c r="C68">
         <v>37</v>
       </c>
-      <c r="D68" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>19</v>
       </c>
-      <c r="B69">
-        <v>3</v>
+      <c r="B69" t="s">
+        <v>4</v>
       </c>
       <c r="C69">
         <v>3</v>
       </c>
-      <c r="D69" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>15</v>
       </c>
-      <c r="B70">
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+      <c r="D70">
         <v>5</v>
       </c>
-      <c r="C70">
-        <v>6</v>
-      </c>
-      <c r="D70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>13</v>
       </c>
-      <c r="B71">
-        <v>0</v>
+      <c r="B71" t="s">
+        <v>4</v>
       </c>
       <c r="C71">
         <v>43</v>
       </c>
-      <c r="D71" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>29</v>
       </c>
-      <c r="B72">
-        <v>1</v>
+      <c r="B72" t="s">
+        <v>4</v>
       </c>
       <c r="C72">
         <v>22</v>
       </c>
-      <c r="D72" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>25</v>
       </c>
-      <c r="B73">
-        <v>1</v>
+      <c r="B73" t="s">
+        <v>4</v>
       </c>
       <c r="C73">
         <v>34</v>
       </c>
-      <c r="D73" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>19</v>
       </c>
-      <c r="B74">
-        <v>0</v>
+      <c r="B74" t="s">
+        <v>4</v>
       </c>
       <c r="C74">
         <v>41</v>
       </c>
-      <c r="D74" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>16</v>
       </c>
-      <c r="B75">
-        <v>0</v>
+      <c r="B75" t="s">
+        <v>4</v>
       </c>
       <c r="C75">
         <v>10</v>
       </c>
-      <c r="D75" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>36</v>
       </c>
-      <c r="B76">
+      <c r="B76" t="s">
         <v>4</v>
       </c>
       <c r="C76">
         <v>5</v>
       </c>
-      <c r="D76" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>8</v>
       </c>
-      <c r="B77">
-        <v>0</v>
+      <c r="B77" t="s">
+        <v>4</v>
       </c>
       <c r="C77">
         <v>17</v>
       </c>
-      <c r="D77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>22</v>
       </c>
-      <c r="B78">
-        <v>0</v>
+      <c r="B78" t="s">
+        <v>4</v>
       </c>
       <c r="C78">
         <v>30</v>
       </c>
-      <c r="D78" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>37</v>
       </c>
-      <c r="B79">
+      <c r="B79" t="s">
         <v>4</v>
       </c>
       <c r="C79">
         <v>4</v>
       </c>
-      <c r="D79" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>28</v>
       </c>
-      <c r="B80">
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
         <v>5</v>
       </c>
-      <c r="C80">
-        <v>1</v>
-      </c>
-      <c r="D80" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>29</v>
       </c>
-      <c r="B81">
-        <v>0</v>
+      <c r="B81" t="s">
+        <v>18</v>
       </c>
       <c r="C81">
         <v>9</v>
       </c>
-      <c r="D81" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>24</v>
       </c>
-      <c r="B82">
-        <v>0</v>
+      <c r="B82" t="s">
+        <v>6</v>
       </c>
       <c r="C82">
         <v>54</v>
       </c>
-      <c r="D82" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>14</v>
       </c>
-      <c r="B83">
-        <v>1</v>
+      <c r="B83" t="s">
+        <v>6</v>
       </c>
       <c r="C83">
         <v>17</v>
       </c>
-      <c r="D83" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>9</v>
       </c>
-      <c r="B84">
-        <v>3</v>
+      <c r="B84" t="s">
+        <v>6</v>
       </c>
       <c r="C84">
         <v>45</v>
       </c>
-      <c r="D84" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>17</v>
       </c>
-      <c r="B85">
-        <v>0</v>
+      <c r="B85" t="s">
+        <v>6</v>
       </c>
       <c r="C85">
         <v>80</v>
       </c>
-      <c r="D85" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>13</v>
       </c>
-      <c r="B86">
-        <v>0</v>
+      <c r="B86" t="s">
+        <v>6</v>
       </c>
       <c r="C86">
         <v>89</v>
       </c>
-      <c r="D86" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>5</v>
       </c>
-      <c r="B87">
-        <v>0</v>
+      <c r="B87" t="s">
+        <v>6</v>
       </c>
       <c r="C87">
         <v>20</v>
       </c>
-      <c r="D87" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>38</v>
       </c>
-      <c r="B88">
-        <v>1</v>
+      <c r="B88" t="s">
+        <v>6</v>
       </c>
       <c r="C88">
         <v>20</v>
       </c>
-      <c r="D88" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>34</v>
       </c>
-      <c r="B89">
+      <c r="B89" t="s">
         <v>6</v>
       </c>
       <c r="C89">
         <v>2</v>
       </c>
-      <c r="D89" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>39</v>
       </c>
-      <c r="B90">
-        <v>0</v>
+      <c r="B90" t="s">
+        <v>6</v>
       </c>
       <c r="C90">
         <v>28</v>
       </c>
-      <c r="D90" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>11</v>
       </c>
-      <c r="B91">
-        <v>0</v>
+      <c r="B91" t="s">
+        <v>4</v>
       </c>
       <c r="C91">
         <v>36</v>
       </c>
-      <c r="D91" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>35</v>
       </c>
-      <c r="B92">
-        <v>2</v>
+      <c r="B92" t="s">
+        <v>4</v>
       </c>
       <c r="C92">
         <v>15</v>
       </c>
-      <c r="D92" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>40</v>
       </c>
-      <c r="B93">
-        <v>2</v>
+      <c r="B93" t="s">
+        <v>4</v>
       </c>
       <c r="C93">
         <v>12</v>
       </c>
-      <c r="D93" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>41</v>
       </c>
-      <c r="B94">
-        <v>2</v>
+      <c r="B94" t="s">
+        <v>4</v>
       </c>
       <c r="C94">
         <v>9</v>
       </c>
-      <c r="D94" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>42</v>
       </c>
-      <c r="B95">
-        <v>0</v>
+      <c r="B95" t="s">
+        <v>4</v>
       </c>
       <c r="C95">
         <v>21</v>
       </c>
-      <c r="D95" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>12</v>
       </c>
-      <c r="B96">
-        <v>2</v>
+      <c r="B96" t="s">
+        <v>4</v>
       </c>
       <c r="C96">
         <v>9</v>
       </c>
-      <c r="D96" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>21</v>
       </c>
-      <c r="B97">
-        <v>1</v>
+      <c r="B97" t="s">
+        <v>4</v>
       </c>
       <c r="C97">
         <v>29</v>
       </c>
-      <c r="D97" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>30</v>
       </c>
-      <c r="B98">
-        <v>3</v>
+      <c r="B98" t="s">
+        <v>4</v>
       </c>
       <c r="C98">
         <v>33</v>
       </c>
-      <c r="D98" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>30</v>
       </c>
-      <c r="B99">
-        <v>1</v>
+      <c r="B99" t="s">
+        <v>4</v>
       </c>
       <c r="C99">
         <v>34</v>
       </c>
-      <c r="D99" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>22</v>
       </c>
-      <c r="B100">
-        <v>2</v>
+      <c r="B100" t="s">
+        <v>4</v>
       </c>
       <c r="C100">
         <v>7</v>
       </c>
-      <c r="D100" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>43</v>
       </c>
-      <c r="B101">
-        <v>0</v>
+      <c r="B101" t="s">
+        <v>4</v>
       </c>
       <c r="C101">
         <v>9</v>
       </c>
-      <c r="D101" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>30</v>
       </c>
-      <c r="B102">
-        <v>3</v>
+      <c r="B102" t="s">
+        <v>4</v>
       </c>
       <c r="C102">
         <v>18</v>
       </c>
-      <c r="D102" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>14</v>
       </c>
-      <c r="B103">
+      <c r="B103" t="s">
         <v>4</v>
       </c>
       <c r="C103">
         <v>15</v>
       </c>
-      <c r="D103" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>10</v>
       </c>
-      <c r="B104">
-        <v>0</v>
+      <c r="B104" t="s">
+        <v>4</v>
       </c>
       <c r="C104">
         <v>26</v>
       </c>
-      <c r="D104" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>9</v>
       </c>
-      <c r="B105">
-        <v>2</v>
+      <c r="B105" t="s">
+        <v>4</v>
       </c>
       <c r="C105">
         <v>25</v>
       </c>
-      <c r="D105" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>22</v>
       </c>
-      <c r="B106">
-        <v>0</v>
+      <c r="B106" t="s">
+        <v>4</v>
       </c>
       <c r="C106">
         <v>36</v>
       </c>
-      <c r="D106" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>23</v>
       </c>
-      <c r="B107">
-        <v>6</v>
+      <c r="B107" t="s">
+        <v>4</v>
       </c>
       <c r="C107">
         <v>15</v>
       </c>
-      <c r="D107" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D107">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>25</v>
       </c>
-      <c r="B108">
-        <v>0</v>
+      <c r="B108" t="s">
+        <v>4</v>
       </c>
       <c r="C108">
         <v>17</v>
       </c>
-      <c r="D108" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>34</v>
       </c>
-      <c r="B109">
-        <v>0</v>
+      <c r="B109" t="s">
+        <v>4</v>
       </c>
       <c r="C109">
         <v>22</v>
       </c>
-      <c r="D109" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>35</v>
       </c>
-      <c r="B110">
-        <v>0</v>
+      <c r="B110" t="s">
+        <v>4</v>
       </c>
       <c r="C110">
         <v>10</v>
       </c>
-      <c r="D110" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>30</v>
       </c>
-      <c r="B111">
-        <v>1</v>
+      <c r="B111" t="s">
+        <v>4</v>
       </c>
       <c r="C111">
         <v>48</v>
       </c>
-      <c r="D111" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>10</v>
       </c>
-      <c r="B112">
-        <v>0</v>
+      <c r="B112" t="s">
+        <v>4</v>
       </c>
       <c r="C112">
         <v>46</v>
       </c>
-      <c r="D112" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>8</v>
       </c>
-      <c r="B113">
-        <v>0</v>
+      <c r="B113" t="s">
+        <v>4</v>
       </c>
       <c r="C113">
         <v>47</v>
       </c>
-      <c r="D113" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>37</v>
       </c>
-      <c r="B114">
-        <v>1</v>
+      <c r="B114" t="s">
+        <v>4</v>
       </c>
       <c r="C114">
         <v>22</v>
       </c>
-      <c r="D114" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>13</v>
       </c>
-      <c r="B115">
-        <v>1</v>
+      <c r="B115" t="s">
+        <v>4</v>
       </c>
       <c r="C115">
         <v>47</v>
       </c>
-      <c r="D115" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>10</v>
       </c>
-      <c r="B116">
-        <v>1</v>
+      <c r="B116" t="s">
+        <v>4</v>
       </c>
       <c r="C116">
         <v>24</v>
       </c>
-      <c r="D116" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>14</v>
       </c>
-      <c r="B117">
-        <v>0</v>
+      <c r="B117" t="s">
+        <v>4</v>
       </c>
       <c r="C117">
         <v>26</v>
       </c>
-      <c r="D117" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>17</v>
       </c>
-      <c r="B118">
-        <v>8</v>
+      <c r="B118" t="s">
+        <v>18</v>
       </c>
       <c r="C118">
         <v>2</v>
       </c>
-      <c r="D118" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D118">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>15</v>
       </c>
-      <c r="B119">
+      <c r="B119" t="s">
         <v>18</v>
       </c>
       <c r="C119">
         <v>2</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119">
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>30</v>
       </c>
-      <c r="B120">
+      <c r="B120" t="s">
         <v>18</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120">
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>7</v>
       </c>
-      <c r="B121">
+      <c r="B121" t="s">
+        <v>18</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
         <v>26</v>
       </c>
-      <c r="C121">
-        <v>0</v>
-      </c>
-      <c r="D121" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>14</v>
       </c>
-      <c r="B122">
-        <v>5</v>
+      <c r="B122" t="s">
+        <v>18</v>
       </c>
       <c r="C122">
         <v>11</v>
       </c>
-      <c r="D122" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>10</v>
       </c>
-      <c r="B123">
-        <v>2</v>
+      <c r="B123" t="s">
+        <v>4</v>
       </c>
       <c r="C123">
         <v>7</v>
       </c>
-      <c r="D123" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>9</v>
       </c>
-      <c r="B124">
-        <v>2</v>
+      <c r="B124" t="s">
+        <v>4</v>
       </c>
       <c r="C124">
         <v>30</v>
       </c>
-      <c r="D124" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>15</v>
       </c>
-      <c r="B125">
-        <v>3</v>
+      <c r="B125" t="s">
+        <v>4</v>
       </c>
       <c r="C125">
         <v>38</v>
       </c>
-      <c r="D125" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>30</v>
       </c>
-      <c r="B126">
-        <v>0</v>
+      <c r="B126" t="s">
+        <v>4</v>
       </c>
       <c r="C126">
         <v>41</v>
       </c>
-      <c r="D126" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>23</v>
       </c>
-      <c r="B127">
-        <v>2</v>
+      <c r="B127" t="s">
+        <v>4</v>
       </c>
       <c r="C127">
         <v>33</v>
       </c>
-      <c r="D127" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>13</v>
       </c>
-      <c r="B128">
-        <v>0</v>
+      <c r="B128" t="s">
+        <v>4</v>
       </c>
       <c r="C128">
         <v>27</v>
       </c>
-      <c r="D128" t="s">
-        <v>4</v>
+      <c r="D128">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>